<commit_message>
Update DNS records spreadsheet
</commit_message>
<xml_diff>
--- a/DNS-RECORDS.xlsx
+++ b/DNS-RECORDS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ann\Git\cross-stitch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6996F452-5FB3-4926-86D2-0A0A33B470A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB000E1-58F0-4A72-9832-D023CB428AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="825" windowWidth="29100" windowHeight="14100" xr2:uid="{DD7B5853-2122-4414-9A70-99F176C879D4}"/>
+    <workbookView xWindow="120" yWindow="1125" windowWidth="28800" windowHeight="14100" xr2:uid="{DD7B5853-2122-4414-9A70-99F176C879D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="72">
   <si>
     <t>Record name</t>
   </si>
@@ -226,13 +226,28 @@
   </si>
   <si>
     <t>CROSS-STITCH-PATTERN.NET</t>
+  </si>
+  <si>
+    <t>Current ALB DNS name</t>
+  </si>
+  <si>
+    <t>Current ACM certificate ARN</t>
+  </si>
+  <si>
+    <t>Current ALB HTTPS security policy</t>
+  </si>
+  <si>
+    <t>arn:aws:acm:us-east-1:358174257684:certificate/8c0f050c-8a28-442f-83ed-e496eda2f04f</t>
+  </si>
+  <si>
+    <t>ELBSecurityPolicy-TLS13-1-2-2021-06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +280,17 @@
       <color theme="4"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0F141A"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -286,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -300,16 +326,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -626,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71E1B90-8906-406D-A373-40905B6F0577}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,7 +670,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="1"/>
@@ -657,31 +687,31 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -750,82 +780,82 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="D5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="7">
         <v>172800</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="6" t="s">
+      <c r="I5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -954,7 +984,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
         <v>66</v>
       </c>
     </row>
@@ -962,31 +992,31 @@
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1088,82 +1118,82 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="D19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>17</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="7">
         <v>172800</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K19" s="6" t="s">
+      <c r="I19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
       <c r="G20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
       <c r="G22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
@@ -1199,82 +1229,82 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="D24" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="7" t="s">
         <v>17</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="7">
         <v>300</v>
       </c>
-      <c r="I24" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K24" s="6" t="s">
+      <c r="I24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
       <c r="G25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
       <c r="G26" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
       <c r="G27" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -1705,28 +1735,32 @@
         <v>13</v>
       </c>
     </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="I19:I22"/>
-    <mergeCell ref="J19:J22"/>
-    <mergeCell ref="K19:K22"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="H19:H22"/>
     <mergeCell ref="I5:I8"/>
     <mergeCell ref="J5:J8"/>
     <mergeCell ref="K5:K8"/>
@@ -1737,6 +1771,26 @@
     <mergeCell ref="E5:E8"/>
     <mergeCell ref="F5:F8"/>
     <mergeCell ref="H5:H8"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="I19:I22"/>
+    <mergeCell ref="J19:J22"/>
+    <mergeCell ref="K19:K22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>